<commit_message>
New layout of Event datastructure in database, send events to database using a Java object instead of horrible child stuff
</commit_message>
<xml_diff>
--- a/DatabaseFields.xlsx
+++ b/DatabaseFields.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexander/Documents/workspaceAndroid/mobEvent/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="27800" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Users</t>
   </si>
@@ -74,9 +86,6 @@
     <t>UniqueEventPicture</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>OwnerOfTheEvent</t>
   </si>
   <si>
@@ -108,6 +117,24 @@
   </si>
   <si>
     <t>ytryt,asd,asfgfds,asdasd</t>
+  </si>
+  <si>
+    <t>StartTime</t>
+  </si>
+  <si>
+    <t>EndTime</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Map&lt;String, Boolean&gt;</t>
+  </si>
+  <si>
+    <t>asfasdafsfasdasd (EUID)</t>
   </si>
 </sst>
 </file>
@@ -151,7 +178,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -164,7 +191,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-Design">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -206,12 +233,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -241,12 +268,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -450,25 +477,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:O19"/>
+  <dimension ref="C6:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.5" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="33.28515625" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="33.33203125" customWidth="1"/>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="14" max="14" width="16.6640625" customWidth="1"/>
+    <col min="17" max="17" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -476,35 +503,44 @@
         <v>4</v>
       </c>
       <c r="M6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
       <c r="I7" t="s">
         <v>5</v>
       </c>
       <c r="J7">
         <v>104</v>
       </c>
+      <c r="K7" t="s">
+        <v>32</v>
+      </c>
       <c r="N7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O7">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
       </c>
       <c r="I8" t="s">
         <v>7</v>
@@ -512,27 +548,39 @@
       <c r="J8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
       </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
       <c r="I9" t="s">
         <v>8</v>
       </c>
       <c r="J9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
       </c>
       <c r="I10" t="s">
         <v>6</v>
@@ -540,71 +588,112 @@
       <c r="J10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.2">
       <c r="I11" t="s">
         <v>12</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.2">
       <c r="I12" t="s">
         <v>14</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.2">
       <c r="I13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.2">
       <c r="I14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.2">
       <c r="I15" t="s">
         <v>18</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="K15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.2">
       <c r="I16" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="J16" s="2">
         <v>0.875</v>
       </c>
-    </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I17" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1</v>
+      </c>
+      <c r="K17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I19" t="s">
+      <c r="K19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>30</v>
+      <c r="K20" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>